<commit_message>
find bug with parse mode. befor fix
</commit_message>
<xml_diff>
--- a/workbook1.xlsx
+++ b/workbook1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demydenko.ay\Downloads\Комп'ютер\tmp\Python\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demydenko.ay\Downloads\Комп'ютер\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$I$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">sheet2!$A$1:$H$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">sheet2!$A$1:$G$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="256">
   <si>
     <t>Поверх</t>
   </si>
@@ -608,6 +608,195 @@
   </si>
   <si>
     <t>V U</t>
+  </si>
+  <si>
+    <t>Brunetka_Kiev</t>
+  </si>
+  <si>
+    <t>AllusiaV</t>
+  </si>
+  <si>
+    <t>Татьяна</t>
+  </si>
+  <si>
+    <t>Natali</t>
+  </si>
+  <si>
+    <t>Valexan</t>
+  </si>
+  <si>
+    <t>Євген</t>
+  </si>
+  <si>
+    <t>Український</t>
+  </si>
+  <si>
+    <t>Рог</t>
+  </si>
+  <si>
+    <t>Tk</t>
+  </si>
+  <si>
+    <t>Natalia</t>
+  </si>
+  <si>
+    <t>Ov</t>
+  </si>
+  <si>
+    <t>toropovskii</t>
+  </si>
+  <si>
+    <t>Евгений</t>
+  </si>
+  <si>
+    <t>Антоничев</t>
+  </si>
+  <si>
+    <t>alexey</t>
+  </si>
+  <si>
+    <t>Влада</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Maas</t>
+  </si>
+  <si>
+    <t>DashFox</t>
+  </si>
+  <si>
+    <t>#nobody#</t>
+  </si>
+  <si>
+    <t>Oleksii</t>
+  </si>
+  <si>
+    <t>Дарина</t>
+  </si>
+  <si>
+    <t>Максим</t>
+  </si>
+  <si>
+    <t>Dmytro</t>
+  </si>
+  <si>
+    <t>M.S K.</t>
+  </si>
+  <si>
+    <t>Nataly</t>
+  </si>
+  <si>
+    <t>Volk</t>
+  </si>
+  <si>
+    <t>Yarik</t>
+  </si>
+  <si>
+    <t>Компаниец</t>
+  </si>
+  <si>
+    <t>Ponomarenko</t>
+  </si>
+  <si>
+    <t>Goloborodko</t>
+  </si>
+  <si>
+    <t>Zaichenko</t>
+  </si>
+  <si>
+    <t>Dmitriv</t>
+  </si>
+  <si>
+    <t>Kudryl</t>
+  </si>
+  <si>
+    <t>Губарев</t>
+  </si>
+  <si>
+    <t>Инна</t>
+  </si>
+  <si>
+    <t>Karpiuk</t>
+  </si>
+  <si>
+    <t>Stepchencko</t>
+  </si>
+  <si>
+    <t>Панюта</t>
+  </si>
+  <si>
+    <t>Sadovnichenko</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Tytarenko</t>
+  </si>
+  <si>
+    <t>Vasyliuk</t>
+  </si>
+  <si>
+    <t>Gus</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Василенко</t>
+  </si>
+  <si>
+    <t>Tkachenko</t>
+  </si>
+  <si>
+    <t>Zhuravlov</t>
+  </si>
+  <si>
+    <t>Коваленко</t>
+  </si>
+  <si>
+    <t>Vladimir</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Vlad</t>
+  </si>
+  <si>
+    <t>Oksana</t>
+  </si>
+  <si>
+    <t>Igor</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Elena</t>
+  </si>
+  <si>
+    <t>Ирина</t>
+  </si>
+  <si>
+    <t>Zoya</t>
+  </si>
+  <si>
+    <t>Svitlana</t>
+  </si>
+  <si>
+    <t>Aleksei</t>
+  </si>
+  <si>
+    <t>Сергей</t>
+  </si>
+  <si>
+    <t>Анна</t>
+  </si>
+  <si>
+    <t>Irenidka</t>
   </si>
 </sst>
 </file>
@@ -638,12 +827,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -659,12 +854,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -692,6 +888,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:H75" totalsRowShown="0">
+  <autoFilter ref="A1:H75"/>
+  <tableColumns count="8">
+    <tableColumn id="8" name="id"/>
+    <tableColumn id="5" name="Username"/>
+    <tableColumn id="6" name="Name"/>
+    <tableColumn id="7" name="Last Name"/>
+    <tableColumn id="10" name="House"/>
+    <tableColumn id="4" name="Секція"/>
+    <tableColumn id="3" name="Поверх"/>
+    <tableColumn id="9" name="Apartment"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2006,750 +2219,1530 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>585560698</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>103550065</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>585561671</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>500967975</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>347004923</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>549546870</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>274285845</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>505806745</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>624864496</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>504482638</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>717646402</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>370783649</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>445522924</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>545731142</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>454337</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>436029137</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>274285845</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>516954108</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>771074406</v>
+      </c>
+      <c r="C20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>363569450</v>
+      </c>
+      <c r="C21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>254281293</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>373048822</v>
+      </c>
+      <c r="B23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>874094941</v>
+      </c>
+      <c r="B24" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" t="s">
+        <v>183</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>473050491</v>
+      </c>
+      <c r="C25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>366448887</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2">
-        <v>585560698</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>422485737</v>
+      </c>
+      <c r="B27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>147781235</v>
+      </c>
+      <c r="B28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" t="s">
+        <v>192</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>524701027</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E29" s="5">
+        <v>3</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>3</v>
+      </c>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>607063192</v>
+      </c>
+      <c r="C30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>565907125</v>
+      </c>
+      <c r="C31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>864063790</v>
+      </c>
+      <c r="C32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" t="s">
+        <v>206</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>477006923</v>
+      </c>
+      <c r="C33" t="s">
+        <v>207</v>
+      </c>
+      <c r="D33" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>704320564</v>
+      </c>
+      <c r="C34" t="s">
+        <v>195</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>749432167</v>
+      </c>
+      <c r="C35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" t="s">
+        <v>199</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>510073320</v>
+      </c>
+      <c r="C36" t="s">
+        <v>208</v>
+      </c>
+      <c r="D36" t="s">
+        <v>200</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>455465677</v>
+      </c>
+      <c r="C37" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>365729530</v>
+      </c>
+      <c r="C38" t="s">
+        <v>209</v>
+      </c>
+      <c r="D38" t="s">
+        <v>201</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>828650261</v>
+      </c>
+      <c r="C39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>752256435</v>
+      </c>
+      <c r="C40" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" t="s">
+        <v>219</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>433650942</v>
+      </c>
+      <c r="C41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D41" t="s">
+        <v>219</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>431757638</v>
+      </c>
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>489677484</v>
+      </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" t="s">
+        <v>221</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>450812589</v>
+      </c>
+      <c r="C44" t="s">
+        <v>243</v>
+      </c>
+      <c r="D44" t="s">
+        <v>222</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>206604359</v>
+      </c>
+      <c r="C45" t="s">
+        <v>244</v>
+      </c>
+      <c r="D45" t="s">
+        <v>223</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>568932031</v>
+      </c>
+      <c r="C46" t="s">
+        <v>245</v>
+      </c>
+      <c r="D46" t="s">
+        <v>224</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>200189699</v>
+      </c>
+      <c r="C47" t="s">
+        <v>246</v>
+      </c>
+      <c r="D47" t="s">
+        <v>225</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>477005192</v>
+      </c>
+      <c r="C48" t="s">
+        <v>242</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>641004857</v>
+      </c>
+      <c r="C49" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" t="s">
+        <v>226</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>561985006</v>
+      </c>
+      <c r="C50" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" t="s">
+        <v>227</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>887524089</v>
+      </c>
+      <c r="C51" t="s">
+        <v>228</v>
+      </c>
+      <c r="D51" t="s">
+        <v>228</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>530751630</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>416343237</v>
+      </c>
+      <c r="C53" t="s">
+        <v>247</v>
+      </c>
+      <c r="D53" t="s">
+        <v>229</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>578046576</v>
+      </c>
+      <c r="C54" t="s">
+        <v>248</v>
+      </c>
+      <c r="D54" t="s">
+        <v>230</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>339798113</v>
+      </c>
+      <c r="C55" t="s">
+        <v>249</v>
+      </c>
+      <c r="D55" t="s">
+        <v>231</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>559566230</v>
+      </c>
+      <c r="C56" t="s">
+        <v>210</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>138666641</v>
+      </c>
+      <c r="C57" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" t="s">
+        <v>240</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>16</v>
+      </c>
+      <c r="H57">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>245924770</v>
+      </c>
+      <c r="C58" t="s">
+        <v>175</v>
+      </c>
+      <c r="D58" t="s">
+        <v>232</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <v>4</v>
+      </c>
+      <c r="G58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>391179144</v>
+      </c>
+      <c r="C59" t="s">
+        <v>211</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59">
+        <v>4</v>
+      </c>
+      <c r="G59">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>206604359</v>
+      </c>
+      <c r="C60" t="s">
+        <v>244</v>
+      </c>
+      <c r="D60" t="s">
+        <v>223</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60">
+        <v>5</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>112663442</v>
+      </c>
+      <c r="C61" t="s">
+        <v>212</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61">
+        <v>5</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>673299465</v>
+      </c>
+      <c r="C62" t="s">
+        <v>242</v>
+      </c>
+      <c r="D62" t="s">
+        <v>233</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>5</v>
+      </c>
+      <c r="G62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>439063206</v>
+      </c>
+      <c r="C63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" t="s">
+        <v>234</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="G63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>632792685</v>
+      </c>
+      <c r="C64" t="s">
+        <v>213</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <v>5</v>
+      </c>
+      <c r="G64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>683862590</v>
+      </c>
+      <c r="C65" t="s">
+        <v>250</v>
+      </c>
+      <c r="D65" t="s">
+        <v>235</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <v>5</v>
+      </c>
+      <c r="G65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>404088540</v>
+      </c>
+      <c r="C66" t="s">
+        <v>214</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <v>5</v>
+      </c>
+      <c r="G66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>355228508</v>
+      </c>
+      <c r="C67" t="s">
+        <v>251</v>
+      </c>
+      <c r="D67" t="s">
+        <v>236</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <v>5</v>
+      </c>
+      <c r="G67">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>548854570</v>
+      </c>
+      <c r="C68" t="s">
+        <v>252</v>
+      </c>
+      <c r="D68" t="s">
+        <v>237</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
+      </c>
+      <c r="G68">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>474740230</v>
+      </c>
+      <c r="C69" t="s">
+        <v>253</v>
+      </c>
+      <c r="D69" t="s">
+        <v>238</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>5</v>
+      </c>
+      <c r="G69">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>440205513</v>
+      </c>
+      <c r="C70" t="s">
+        <v>175</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>454013985</v>
+      </c>
+      <c r="C71" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>127141610</v>
+      </c>
+      <c r="C72" t="s">
+        <v>216</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>670212651</v>
+      </c>
+      <c r="C73" t="s">
+        <v>254</v>
+      </c>
+      <c r="D73" t="s">
+        <v>241</v>
+      </c>
+      <c r="E73">
+        <v>4</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>25</v>
+      </c>
+      <c r="H73">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>407058673</v>
+      </c>
+      <c r="C74" t="s">
+        <v>217</v>
+      </c>
+      <c r="E74">
+        <v>4</v>
+      </c>
+      <c r="F74">
+        <v>5</v>
+      </c>
+      <c r="G74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>432126343</v>
+      </c>
+      <c r="C75" t="s">
+        <v>255</v>
+      </c>
+      <c r="D75" t="s">
+        <v>239</v>
+      </c>
+      <c r="E75">
+        <v>4</v>
+      </c>
+      <c r="F75">
+        <v>5</v>
+      </c>
+      <c r="G75">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>103550065</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4">
-        <v>585561671</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5">
-        <v>500967975</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6">
-        <v>347004923</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7">
-        <v>549546870</v>
-      </c>
-      <c r="I7">
-        <v>208</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8">
-        <v>274285845</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9">
-        <v>505806745</v>
-      </c>
-      <c r="I9">
-        <v>219</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10">
-        <v>624864496</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11">
-        <v>504482638</v>
-      </c>
-      <c r="I11">
-        <v>232</v>
-      </c>
-      <c r="J11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12">
-        <v>717646402</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13">
-        <v>370783649</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" t="s">
-        <v>93</v>
-      </c>
-      <c r="H14">
-        <v>445522924</v>
-      </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F15" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15">
-        <v>545731142</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G16" t="s">
-        <v>106</v>
-      </c>
-      <c r="H16">
-        <v>454337</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" t="s">
-        <v>123</v>
-      </c>
-      <c r="G17" t="s">
-        <v>124</v>
-      </c>
-      <c r="H17">
-        <v>436029137</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" t="s">
-        <v>133</v>
-      </c>
-      <c r="G18" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18">
-        <v>274285845</v>
-      </c>
-      <c r="J18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19">
-        <v>11</v>
-      </c>
-      <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G19" t="s">
-        <v>148</v>
-      </c>
-      <c r="H19">
-        <v>516954108</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="D20">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>175</v>
-      </c>
-      <c r="G20" t="s">
-        <v>176</v>
-      </c>
-      <c r="H20">
-        <v>771074406</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="F21" t="s">
-        <v>178</v>
-      </c>
-      <c r="G21" t="s">
-        <v>179</v>
-      </c>
-      <c r="H21">
-        <v>363569450</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>184</v>
-      </c>
-      <c r="F22" t="s">
-        <v>180</v>
-      </c>
-      <c r="H22">
-        <v>254281293</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>14</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>182</v>
-      </c>
-      <c r="F23" t="s">
-        <v>181</v>
-      </c>
-      <c r="G23" t="s">
-        <v>182</v>
-      </c>
-      <c r="H23">
-        <v>373048822</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>185</v>
-      </c>
-      <c r="F24" t="s">
-        <v>183</v>
-      </c>
-      <c r="H24">
-        <v>874094941</v>
-      </c>
-      <c r="I24">
-        <v>620</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="F25" t="s">
-        <v>186</v>
-      </c>
-      <c r="G25" t="s">
-        <v>187</v>
-      </c>
-      <c r="H25">
-        <v>473050491</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <v>7</v>
-      </c>
-      <c r="D26">
-        <v>6</v>
-      </c>
-      <c r="F26" t="s">
-        <v>188</v>
-      </c>
-      <c r="H26">
-        <v>366448887</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>7</v>
-      </c>
-      <c r="D27">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>190</v>
-      </c>
-      <c r="F27" t="s">
-        <v>189</v>
-      </c>
-      <c r="H27">
-        <v>422485737</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>9</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>191</v>
-      </c>
-      <c r="F28" t="s">
-        <v>192</v>
-      </c>
-      <c r="H28">
-        <v>147781235</v>
-      </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H19"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="/im?p=u585560698" display="https://web.telegram.org/ - /im?p=u585560698"/>
-    <hyperlink ref="A3" r:id="rId2" location="/im?p=u103550065" display="https://web.telegram.org/ - /im?p=u103550065"/>
-    <hyperlink ref="A4" r:id="rId3" location="/im?p=u585561671" display="https://web.telegram.org/ - /im?p=u585561671"/>
-    <hyperlink ref="A5" r:id="rId4" location="/im?p=u500967975" display="https://web.telegram.org/ - /im?p=u500967975"/>
-    <hyperlink ref="A6" r:id="rId5" location="/im?p=u347004923" display="https://web.telegram.org/ - /im?p=u347004923"/>
-    <hyperlink ref="A7" r:id="rId6" location="/im?p=u549546870" display="https://web.telegram.org/ - /im?p=u549546870"/>
-    <hyperlink ref="A8" r:id="rId7" location="/im?p=u274285845" display="https://web.telegram.org/ - /im?p=u274285845"/>
-    <hyperlink ref="A9" r:id="rId8" location="/im?p=u505806745" display="https://web.telegram.org/ - /im?p=u505806745"/>
-    <hyperlink ref="A10" r:id="rId9" location="/im?p=u624864496" display="https://web.telegram.org/ - /im?p=u624864496"/>
-    <hyperlink ref="A11" r:id="rId10" location="/im?p=u504482638" display="https://web.telegram.org/ - /im?p=u504482638"/>
-    <hyperlink ref="A12" r:id="rId11" location="/im?p=u717646402" display="https://web.telegram.org/ - /im?p=u717646402"/>
-    <hyperlink ref="A13" r:id="rId12" location="/im?p=u370783649" display="https://web.telegram.org/ - /im?p=u370783649"/>
-    <hyperlink ref="A14" r:id="rId13" location="/im?p=u445522924" display="https://web.telegram.org/ - /im?p=u445522924"/>
-    <hyperlink ref="A15" r:id="rId14" location="/im?p=u545731142" display="https://web.telegram.org/ - /im?p=u545731142"/>
-    <hyperlink ref="A16" r:id="rId15" location="/im?p=u454337" display="https://web.telegram.org/ - /im?p=u454337"/>
-    <hyperlink ref="A17" r:id="rId16" location="/im?p=u436029137" display="https://web.telegram.org/ - /im?p=u436029137"/>
-    <hyperlink ref="A18" r:id="rId17" location="/im?p=u274285845" display="https://web.telegram.org/ - /im?p=u274285845"/>
-    <hyperlink ref="A19" r:id="rId18" location="/im?p=u516954108" display="https://web.telegram.org/ - /im?p=u516954108"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>